<commit_message>
fixed filter date fitur Rekap NG
</commit_message>
<xml_diff>
--- a/storage/template/Export_Rekap_NG_CSH_D05E.xlsx
+++ b/storage/template/Export_Rekap_NG_CSH_D05E.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Sotfware\laravel\avicenna\storage\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F36C3C-F725-4C77-AE63-49FA2F71C314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330256DD-048F-46F3-9C21-440C818B2834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05F26BD9-E112-4214-87F4-B2A2D3F2905B}"/>
   </bookViews>
@@ -301,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -316,18 +316,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -366,11 +354,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -776,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791A0E52-CC1A-4F19-9301-04A76062EC8D}">
   <dimension ref="A17:X1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -799,16 +810,16 @@
   <sheetData>
     <row r="17" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -836,49 +847,49 @@
       <c r="H20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L20" s="18" t="s">
+      <c r="L20" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="11" t="s">
+      <c r="P20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Q20" s="11" t="s">
+      <c r="Q20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R20" s="11" t="s">
+      <c r="R20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S20" s="11" t="s">
+      <c r="S20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T20" s="11" t="s">
+      <c r="T20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="U20" s="11" t="s">
+      <c r="U20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="V20" s="11" t="s">
+      <c r="V20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="W20" s="15" t="s">
+      <c r="W20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="X20" s="17" t="s">
+      <c r="X20" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -891,61 +902,61 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="J21" s="13">
+      <c r="J21" s="9">
         <v>8</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21" s="16">
         <v>1</v>
       </c>
-      <c r="L21" s="19">
+      <c r="L21" s="15">
         <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,L$20)</f>
         <v>0</v>
       </c>
-      <c r="M21" s="14">
+      <c r="M21" s="10">
         <f t="shared" ref="M21:W21" si="0">COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,M$20)</f>
         <v>0</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O21" s="14">
+      <c r="O21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="14">
+      <c r="Q21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R21" s="14">
+      <c r="R21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S21" s="14">
+      <c r="S21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T21" s="14">
+      <c r="T21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U21" s="14">
+      <c r="U21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V21" s="14">
+      <c r="V21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W21" s="16">
+      <c r="W21" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X21" s="21">
+      <c r="X21" s="17">
         <f>SUM(L21:W21)</f>
         <v>0</v>
       </c>
@@ -984,8 +995,8 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -1009,8 +1020,8 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
       <c r="L24"/>
       <c r="M24"/>
       <c r="N24"/>
@@ -1034,8 +1045,8 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
       <c r="L25"/>
       <c r="M25"/>
       <c r="N25"/>
@@ -1059,8 +1070,8 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
       <c r="L26"/>
       <c r="M26"/>
       <c r="N26"/>
@@ -1084,8 +1095,8 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
       <c r="L27"/>
       <c r="M27"/>
       <c r="N27"/>
@@ -1109,8 +1120,8 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
       <c r="L28"/>
       <c r="M28"/>
       <c r="N28"/>
@@ -1134,8 +1145,8 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
       <c r="L29"/>
       <c r="M29"/>
       <c r="N29"/>
@@ -1159,8 +1170,8 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
       <c r="L30"/>
       <c r="M30"/>
       <c r="N30"/>
@@ -1184,8 +1195,8 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
       <c r="L31"/>
       <c r="M31"/>
       <c r="N31"/>
@@ -1209,8 +1220,8 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
       <c r="L32"/>
       <c r="M32"/>
       <c r="N32"/>
@@ -1234,8 +1245,8 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
       <c r="L33"/>
       <c r="M33"/>
       <c r="N33"/>
@@ -1259,8 +1270,8 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
       <c r="L34"/>
       <c r="M34"/>
       <c r="N34"/>
@@ -1284,8 +1295,8 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
       <c r="L35"/>
       <c r="M35"/>
       <c r="N35"/>
@@ -1309,8 +1320,8 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
       <c r="L36"/>
       <c r="M36"/>
       <c r="N36"/>
@@ -1334,8 +1345,8 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
       <c r="L37"/>
       <c r="M37"/>
       <c r="N37"/>
@@ -1359,8 +1370,8 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
       <c r="L38"/>
       <c r="M38"/>
       <c r="N38"/>
@@ -1384,8 +1395,8 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
       <c r="L39"/>
       <c r="M39"/>
       <c r="N39"/>
@@ -1409,8 +1420,8 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
       <c r="L40"/>
       <c r="M40"/>
       <c r="N40"/>
@@ -1434,8 +1445,8 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
       <c r="L41"/>
       <c r="M41"/>
       <c r="N41"/>
@@ -1459,8 +1470,8 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
       <c r="L42"/>
       <c r="M42"/>
       <c r="N42"/>
@@ -1484,8 +1495,8 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43"/>
@@ -1509,8 +1520,8 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
       <c r="L44"/>
       <c r="M44"/>
       <c r="N44"/>
@@ -1534,8 +1545,8 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
       <c r="L45"/>
       <c r="M45"/>
       <c r="N45"/>
@@ -1559,8 +1570,8 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
       <c r="L46"/>
       <c r="M46"/>
       <c r="N46"/>
@@ -1584,8 +1595,8 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
       <c r="L47"/>
       <c r="M47"/>
       <c r="N47"/>
@@ -11325,8 +11336,11 @@
     <mergeCell ref="A18:H18"/>
   </mergeCells>
   <conditionalFormatting sqref="L21:X21">
-    <cfRule type="notContainsText" dxfId="0" priority="1" operator="notContains" text="0">
+    <cfRule type="notContainsText" dxfId="0" priority="2" operator="notContains" text="0">
       <formula>ISERROR(SEARCH("0",L21))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add edit dan delete di fitur Rekap NG
</commit_message>
<xml_diff>
--- a/storage/template/Export_Rekap_NG_CSH_D05E.xlsx
+++ b/storage/template/Export_Rekap_NG_CSH_D05E.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Sotfware\laravel\avicenna\storage\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330256DD-048F-46F3-9C21-440C818B2834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41C1BE9-E0ED-497D-870C-76990B3A7910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05F26BD9-E112-4214-87F4-B2A2D3F2905B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>NO</t>
   </si>
@@ -103,12 +103,54 @@
   <si>
     <t>CSH D05E</t>
   </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>LEAK</t>
+  </si>
+  <si>
+    <t>YOGORE</t>
+  </si>
+  <si>
+    <t>CRACK</t>
+  </si>
+  <si>
+    <t>HARDSPOT</t>
+  </si>
+  <si>
+    <t>DENT</t>
+  </si>
+  <si>
+    <t>OTHERS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +162,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -301,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -336,9 +384,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,7 +412,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -785,9 +844,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791A0E52-CC1A-4F19-9301-04A76062EC8D}">
-  <dimension ref="A17:X1019"/>
+  <dimension ref="A17:AL1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -805,24 +864,26 @@
     <col min="10" max="10" width="10.54296875" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.7265625" style="1" customWidth="1"/>
     <col min="12" max="24" width="8.7265625" style="4"/>
-    <col min="25" max="16384" width="8.7265625" style="1"/>
+    <col min="25" max="34" width="8.7265625" style="1"/>
+    <col min="35" max="35" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="18" t="s">
+    <row r="17" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="20"/>
-    </row>
-    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
@@ -853,7 +914,7 @@
       <c r="K20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="13" t="s">
         <v>8</v>
       </c>
       <c r="M20" s="7" t="s">
@@ -878,26 +939,68 @@
         <v>15</v>
       </c>
       <c r="T20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="W20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="X20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="U20" s="7" t="s">
+      <c r="AC20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="V20" s="7" t="s">
+      <c r="AD20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="W20" s="11" t="s">
+      <c r="AE20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="X20" s="13" t="s">
+      <c r="AF20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL20" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -905,15 +1008,15 @@
       <c r="J21" s="9">
         <v>8</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K21" s="15">
         <v>1</v>
       </c>
-      <c r="L21" s="15">
+      <c r="L21" s="14">
         <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,L$20)</f>
         <v>0</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" ref="M21:W21" si="0">COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,M$20)</f>
+        <f t="shared" ref="M21:AA21" si="0">COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,M$20)</f>
         <v>0</v>
       </c>
       <c r="N21" s="10">
@@ -952,16 +1055,72 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W21" s="12">
+      <c r="W21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X21" s="17">
-        <f>SUM(L21:W21)</f>
+      <c r="X21" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="10">
+        <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="10">
+        <f t="shared" ref="U21:AF21" si="1">COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="10">
+        <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="10">
+        <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,AF$20)</f>
+        <v>0</v>
+      </c>
+      <c r="AG21" s="10">
+        <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,AG$20)</f>
+        <v>0</v>
+      </c>
+      <c r="AH21" s="10">
+        <f t="shared" ref="AH21:AK21" si="2">COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,AH$20)</f>
+        <v>0</v>
+      </c>
+      <c r="AI21" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK21" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL21" s="16">
+        <f>SUM(L21:AK21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -986,7 +1145,7 @@
       <c r="W22"/>
       <c r="X22"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1011,7 +1170,7 @@
       <c r="W23"/>
       <c r="X23"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1036,7 +1195,7 @@
       <c r="W24"/>
       <c r="X24"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1061,7 +1220,7 @@
       <c r="W25"/>
       <c r="X25"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1086,7 +1245,7 @@
       <c r="W26"/>
       <c r="X26"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1111,7 +1270,7 @@
       <c r="W27"/>
       <c r="X27"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1136,7 +1295,7 @@
       <c r="W28"/>
       <c r="X28"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1161,7 +1320,7 @@
       <c r="W29"/>
       <c r="X29"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1186,7 +1345,7 @@
       <c r="W30"/>
       <c r="X30"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1211,7 +1370,7 @@
       <c r="W31"/>
       <c r="X31"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -11335,11 +11494,15 @@
   <mergeCells count="1">
     <mergeCell ref="A18:H18"/>
   </mergeCells>
-  <conditionalFormatting sqref="L21:X21">
-    <cfRule type="notContainsText" dxfId="0" priority="2" operator="notContains" text="0">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="L21:AL21">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="notContainsText" dxfId="1" priority="3" operator="notContains" text="0">
       <formula>ISERROR(SEARCH("0",L21))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>